<commit_message>
commit feature get posts
</commit_message>
<xml_diff>
--- a/Data Files/JsonPlacer.xlsx
+++ b/Data Files/JsonPlacer.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekapangaribuan/Desktop/Automation-Project/katalon-api-placeholder/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB07FBBF-9FBA-6344-A64C-4DD2A7942FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF8BF82-CC29-D04D-BC49-B74EA3159C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="1" xr2:uid="{EF6870CB-0A1F-6642-95A2-8516B2436393}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="2" xr2:uid="{EF6870CB-0A1F-6642-95A2-8516B2436393}"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="1" r:id="rId1"/>
     <sheet name="Post-Delete" sheetId="2" r:id="rId2"/>
+    <sheet name="Get-Post" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>title</t>
   </si>
@@ -73,13 +74,43 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>optio molestias id quia eum</t>
+  </si>
+  <si>
+    <t>doloribus ad provident suscipit at</t>
+  </si>
+  <si>
+    <t>qui consequuntur ducimus possimus quisquam amet similique\nsuscipit porro ipsam amet\neos veritatis officiis exercitationem vel fugit aut necessitatibus totam\nomnis rerum consequatur expedita quidem cumque explicabo</t>
+  </si>
+  <si>
+    <t>a quo magni similique perferendis</t>
+  </si>
+  <si>
+    <t>alias dolor cumque\nimpedit blanditiis non eveniet odio maxime\nblanditiis amet eius quis tempora quia autem rem\na provident perspiciatis quia</t>
+  </si>
+  <si>
+    <t>enim quo cumque</t>
+  </si>
+  <si>
+    <t>ut voluptatum aliquid illo tenetur nemo sequi quo facilis\nipsum rem optio mollitia quas\nvoluptatem eum voluptas qui\nunde omnis voluptatem iure quasi maxime voluptas nam</t>
+  </si>
+  <si>
+    <t>repellendus qui recusandae incidunt voluptates tenetur qui omnis exercitationem</t>
+  </si>
+  <si>
+    <t>error suscipit maxime adipisci consequuntur recusandae\nvoluptas eligendi et est et voluptates\nquia distinctio ab amet quaerat molestiae et vitae\nadipisci impedit sequi nesciunt quis consectetur</t>
+  </si>
+  <si>
+    <t>sss quo et expedita modi cum officia vel magni\ndoloribus qui repudiandae\nvero nisi sit\nquos veniam quod sed accusamus veritatis error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,6 +123,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,8 +151,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFBEC7B-8CD8-E44F-B75C-5005981D3F05}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -546,4 +584,107 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0FCE1F-EF31-284A-9D57-DE9AF6179792}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="115.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>